<commit_message>
Optimizer produces pairing with the highest player preferences.
</commit_message>
<xml_diff>
--- a/Benchmark Tracking Sheet.xlsx
+++ b/Benchmark Tracking Sheet.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\twanb\Documents\NK-Schandom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0EEBA1-43EF-446F-839B-4C5065B4CB40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEDC9622-D1EE-4216-ADBE-B270967A5D73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{95C23759-64AD-4554-B4CD-AFB31BB32783}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{95C23759-64AD-4554-B4CD-AFB31BB32783}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -52,6 +54,57 @@
   </si>
   <si>
     <t>Min match</t>
+  </si>
+  <si>
+    <t>Seed</t>
+  </si>
+  <si>
+    <t>1A</t>
+  </si>
+  <si>
+    <t>WOS</t>
+  </si>
+  <si>
+    <t>TWB</t>
+  </si>
+  <si>
+    <t>Belgisch Bierschaak</t>
+  </si>
+  <si>
+    <t>1B</t>
+  </si>
+  <si>
+    <t>JAS</t>
+  </si>
+  <si>
+    <t>ROS</t>
+  </si>
+  <si>
+    <t>Cilinderschaak</t>
+  </si>
+  <si>
+    <t>2A</t>
+  </si>
+  <si>
+    <t>Chinees Schaken</t>
+  </si>
+  <si>
+    <t>2B</t>
+  </si>
+  <si>
+    <t>Abalone</t>
+  </si>
+  <si>
+    <t>3A</t>
+  </si>
+  <si>
+    <t>Backgammon</t>
+  </si>
+  <si>
+    <t>3B</t>
+  </si>
+  <si>
+    <t>Betoverde doolhof</t>
   </si>
 </sst>
 </file>
@@ -87,9 +140,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,58 +462,271 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37A63F41-6396-4FD6-B354-9362634C4057}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>45398</v>
+      </c>
+      <c r="B2" s="1">
+        <v>29024</v>
+      </c>
+      <c r="C2" s="1">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1">
+        <v>528</v>
+      </c>
+      <c r="E2" s="1">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1">
+        <v>120</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D65EB5D5-505E-42AB-944F-399B6529D89D}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>45398</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2284</v>
+      </c>
+      <c r="C2" s="1">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="D2" s="1">
+        <v>381</v>
+      </c>
+      <c r="E2" s="1">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1">
+        <v>32</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4795ED82-32AF-4B7F-97D9-F7F23E4BD1F3}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1">
+        <v>26</v>
+      </c>
+      <c r="H1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2">
+        <v>26</v>
+      </c>
+      <c r="H2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3">
+        <v>18</v>
+      </c>
+      <c r="H3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4">
+        <v>15</v>
+      </c>
+      <c r="H4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5">
+        <v>10</v>
+      </c>
+      <c r="H5">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>45394</v>
-      </c>
-      <c r="B2">
-        <v>26103</v>
-      </c>
-      <c r="C2">
-        <v>20</v>
-      </c>
-      <c r="D2">
-        <v>475</v>
-      </c>
-      <c r="E2">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="F2">
-        <v>351</v>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6">
+        <v>8</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>